<commit_message>
KepAdatbazis kiegészítése, eseményközlő olvashatóbbá alakítása
- Ellenfelek képeinek feltöltése, a képek elérési címének eltárolása
fájlba
- KepAdatbazis kiegészítése az ellenfelek képeinek lekérdezésével
- A Harcter windowon az ellenfél képe egy random kép lesz az
ellenfeleknek feltöltöttek közül.
- Az eseményközlő betűinek színe megváltoztatva fehér színűvé, hogy
olvashatóbb legyen.
</commit_message>
<xml_diff>
--- a/Raetreon/bin/Debug/Fajlok/DB/hosadatbazis.xlsx
+++ b/Raetreon/bin/Debug/Fajlok/DB/hosadatbazis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19095" windowHeight="5385" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19095" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Harcosok" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Név</t>
   </si>
@@ -57,34 +57,25 @@
     <t>Kep</t>
   </si>
   <si>
-    <t>Images/hoskepek/mordin.jpg</t>
-  </si>
-  <si>
-    <t>Images/hoskepek/zileth.jpg</t>
-  </si>
-  <si>
-    <t>Images/hoskepek/egrar.jpg</t>
-  </si>
-  <si>
-    <t>Images/hoskepek/shue.jpg</t>
-  </si>
-  <si>
-    <t>Images/hoskepek/vloras.jpg</t>
-  </si>
-  <si>
-    <t>Images/hoskepek/rem.jpg</t>
-  </si>
-  <si>
-    <t>Images/hoskepek/nihlah.jpg</t>
-  </si>
-  <si>
-    <t>Images/hoskepek/hini.jpg</t>
-  </si>
-  <si>
-    <t>Images/hoskepek/yesmeh.png</t>
-  </si>
-  <si>
-    <t>Images/hoskepek/nuzan.jpg</t>
+    <t>Images\Karakterek\ellenseg.png</t>
+  </si>
+  <si>
+    <t>Images\Karakterek\ellenseg2.png</t>
+  </si>
+  <si>
+    <t>Images\Karakterek\ellenseg3.png</t>
+  </si>
+  <si>
+    <t>Images\Karakterek\golem1.png</t>
+  </si>
+  <si>
+    <t>Images\Karakterek\golem2.png</t>
+  </si>
+  <si>
+    <t>Images\Karakterek\golem3.png</t>
+  </si>
+  <si>
+    <t>Images\Karakterek\golem4.png</t>
   </si>
 </sst>
 </file>
@@ -419,15 +410,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -496,7 +487,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -559,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -589,7 +580,7 @@
         <v>1000</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -600,7 +591,7 @@
         <v>1000</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -611,7 +602,7 @@
         <v>1000</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>